<commit_message>
FIX - StudentController method createFromCsv
</commit_message>
<xml_diff>
--- a/public/output.xlsx
+++ b/public/output.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="83">
   <si>
     <t>Lista de studiantes</t>
   </si>
@@ -219,6 +219,9 @@
     <t>VILLALTA BALCAZAR</t>
   </si>
   <si>
+    <t>test3</t>
+  </si>
+  <si>
     <t>Fechas</t>
   </si>
   <si>
@@ -261,7 +264,7 @@
     <t>57%</t>
   </si>
   <si>
-    <t>43%</t>
+    <t>14%</t>
   </si>
 </sst>
 </file>
@@ -600,7 +603,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1768,6 +1771,70 @@
       </c>
       <c r="M38">
         <v>1.0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39">
+        <v>123456789</v>
+      </c>
+      <c r="B39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39">
+        <v>0.0</v>
+      </c>
+      <c r="E39">
+        <v>0.0</v>
+      </c>
+      <c r="F39">
+        <v>0.0</v>
+      </c>
+      <c r="G39">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40">
+        <v>123456789</v>
+      </c>
+      <c r="B40" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0.0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0.0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>0.0</v>
+      </c>
+      <c r="M40">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -1797,7 +1864,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1810,10 +1877,10 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -1827,37 +1894,37 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -1871,21 +1938,21 @@
         <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H12"/>
       <c r="I12"/>
       <c r="J12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K12">
         <v>5</v>
@@ -1897,7 +1964,7 @@
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -1911,33 +1978,33 @@
         <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E13" t="s">
         <v>76</v>
       </c>
       <c r="F13" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G13" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H13"/>
       <c r="I13"/>
       <c r="J13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13">
         <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -1951,30 +2018,30 @@
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" t="s">
         <v>77</v>
       </c>
-      <c r="F14" t="s">
-        <v>76</v>
-      </c>
       <c r="G14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H14"/>
       <c r="I14"/>
       <c r="J14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L14">
         <v>1</v>
       </c>
       <c r="M14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N14" t="s">
         <v>80</v>
@@ -1991,21 +2058,21 @@
         <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E15" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F15" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G15" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H15"/>
       <c r="I15"/>
       <c r="J15" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K15">
         <v>4</v>
@@ -2017,7 +2084,7 @@
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -2031,30 +2098,30 @@
         <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E16" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" t="s">
         <v>77</v>
       </c>
-      <c r="F16" t="s">
-        <v>76</v>
-      </c>
       <c r="G16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H16"/>
       <c r="I16"/>
       <c r="J16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L16">
         <v>1</v>
       </c>
       <c r="M16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N16" t="s">
         <v>80</v>
@@ -2071,30 +2138,30 @@
         <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E17" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" t="s">
         <v>77</v>
       </c>
-      <c r="F17" t="s">
-        <v>76</v>
-      </c>
       <c r="G17" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H17"/>
       <c r="I17"/>
       <c r="J17" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L17">
         <v>1</v>
       </c>
       <c r="M17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17" t="s">
         <v>80</v>
@@ -2111,30 +2178,30 @@
         <v>26</v>
       </c>
       <c r="D18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E18" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" t="s">
         <v>77</v>
       </c>
-      <c r="F18" t="s">
-        <v>76</v>
-      </c>
       <c r="G18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H18"/>
       <c r="I18"/>
       <c r="J18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L18">
         <v>1</v>
       </c>
       <c r="M18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N18" t="s">
         <v>80</v>
@@ -2151,30 +2218,30 @@
         <v>28</v>
       </c>
       <c r="D19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F19" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H19"/>
       <c r="I19"/>
       <c r="J19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N19" t="s">
         <v>81</v>
@@ -2191,33 +2258,33 @@
         <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E20" t="s">
         <v>76</v>
       </c>
       <c r="F20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H20"/>
       <c r="I20"/>
       <c r="J20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K20">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M20">
         <v>0</v>
       </c>
       <c r="N20" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -2231,21 +2298,21 @@
         <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F21" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H21"/>
       <c r="I21"/>
       <c r="J21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K21">
         <v>4</v>
@@ -2257,7 +2324,7 @@
         <v>0</v>
       </c>
       <c r="N21" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -2271,33 +2338,33 @@
         <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E22" t="s">
         <v>76</v>
       </c>
       <c r="F22" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G22" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H22"/>
       <c r="I22"/>
       <c r="J22" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M22">
         <v>0</v>
       </c>
       <c r="N22" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -2311,21 +2378,21 @@
         <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E23" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F23" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G23" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H23"/>
       <c r="I23"/>
       <c r="J23" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K23">
         <v>4</v>
@@ -2337,7 +2404,7 @@
         <v>1</v>
       </c>
       <c r="N23" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -2351,30 +2418,30 @@
         <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E24" t="s">
+        <v>76</v>
+      </c>
+      <c r="F24" t="s">
+        <v>76</v>
+      </c>
+      <c r="G24" t="s">
         <v>77</v>
-      </c>
-      <c r="F24" t="s">
-        <v>75</v>
-      </c>
-      <c r="G24" t="s">
-        <v>76</v>
       </c>
       <c r="H24"/>
       <c r="I24"/>
       <c r="J24" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L24">
         <v>1</v>
       </c>
       <c r="M24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N24" t="s">
         <v>80</v>
@@ -2391,30 +2458,30 @@
         <v>40</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E25" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" t="s">
         <v>77</v>
       </c>
-      <c r="F25" t="s">
-        <v>76</v>
-      </c>
       <c r="G25" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H25"/>
       <c r="I25"/>
       <c r="J25" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L25">
         <v>1</v>
       </c>
       <c r="M25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N25" t="s">
         <v>80</v>
@@ -2431,30 +2498,30 @@
         <v>42</v>
       </c>
       <c r="D26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E26" t="s">
+        <v>76</v>
+      </c>
+      <c r="F26" t="s">
         <v>77</v>
       </c>
-      <c r="F26" t="s">
-        <v>76</v>
-      </c>
       <c r="G26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H26"/>
       <c r="I26"/>
       <c r="J26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L26">
         <v>1</v>
       </c>
       <c r="M26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N26" t="s">
         <v>80</v>
@@ -2471,21 +2538,21 @@
         <v>44</v>
       </c>
       <c r="D27" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E27" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F27" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G27" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H27"/>
       <c r="I27"/>
       <c r="J27" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K27">
         <v>5</v>
@@ -2497,7 +2564,7 @@
         <v>0</v>
       </c>
       <c r="N27" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:14">
@@ -2511,21 +2578,21 @@
         <v>46</v>
       </c>
       <c r="D28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H28"/>
       <c r="I28"/>
       <c r="J28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K28">
         <v>4</v>
@@ -2537,7 +2604,7 @@
         <v>0</v>
       </c>
       <c r="N28" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -2551,21 +2618,21 @@
         <v>48</v>
       </c>
       <c r="D29" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E29" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F29" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G29" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H29"/>
       <c r="I29"/>
       <c r="J29" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K29">
         <v>4</v>
@@ -2577,7 +2644,7 @@
         <v>0</v>
       </c>
       <c r="N29" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -2591,21 +2658,21 @@
         <v>50</v>
       </c>
       <c r="D30" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E30" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F30" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G30" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H30"/>
       <c r="I30"/>
       <c r="J30" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K30">
         <v>5</v>
@@ -2617,7 +2684,7 @@
         <v>0</v>
       </c>
       <c r="N30" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:14">
@@ -2631,30 +2698,30 @@
         <v>52</v>
       </c>
       <c r="D31" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E31" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" t="s">
+        <v>76</v>
+      </c>
+      <c r="G31" t="s">
         <v>77</v>
-      </c>
-      <c r="F31" t="s">
-        <v>75</v>
-      </c>
-      <c r="G31" t="s">
-        <v>76</v>
       </c>
       <c r="H31"/>
       <c r="I31"/>
       <c r="J31" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L31">
         <v>1</v>
       </c>
       <c r="M31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N31" t="s">
         <v>80</v>
@@ -2671,30 +2738,30 @@
         <v>54</v>
       </c>
       <c r="D32" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E32" t="s">
+        <v>76</v>
+      </c>
+      <c r="F32" t="s">
         <v>77</v>
       </c>
-      <c r="F32" t="s">
-        <v>76</v>
-      </c>
       <c r="G32" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H32"/>
       <c r="I32"/>
       <c r="J32" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L32">
         <v>1</v>
       </c>
       <c r="M32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N32" t="s">
         <v>80</v>
@@ -2711,30 +2778,30 @@
         <v>56</v>
       </c>
       <c r="D33" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E33" t="s">
+        <v>76</v>
+      </c>
+      <c r="F33" t="s">
         <v>77</v>
       </c>
-      <c r="F33" t="s">
-        <v>76</v>
-      </c>
       <c r="G33" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H33"/>
       <c r="I33"/>
       <c r="J33" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K33">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L33">
         <v>1</v>
       </c>
       <c r="M33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N33" t="s">
         <v>80</v>
@@ -2751,30 +2818,30 @@
         <v>58</v>
       </c>
       <c r="D34" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E34" t="s">
+        <v>76</v>
+      </c>
+      <c r="F34" t="s">
         <v>77</v>
       </c>
-      <c r="F34" t="s">
-        <v>76</v>
-      </c>
       <c r="G34" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H34"/>
       <c r="I34"/>
       <c r="J34" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K34">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L34">
         <v>1</v>
       </c>
       <c r="M34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N34" t="s">
         <v>80</v>
@@ -2791,30 +2858,30 @@
         <v>60</v>
       </c>
       <c r="D35" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E35" t="s">
+        <v>76</v>
+      </c>
+      <c r="F35" t="s">
         <v>77</v>
       </c>
-      <c r="F35" t="s">
-        <v>76</v>
-      </c>
       <c r="G35" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H35"/>
       <c r="I35"/>
       <c r="J35" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K35">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L35">
         <v>1</v>
       </c>
       <c r="M35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N35" t="s">
         <v>80</v>
@@ -2831,30 +2898,30 @@
         <v>62</v>
       </c>
       <c r="D36" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E36" t="s">
+        <v>76</v>
+      </c>
+      <c r="F36" t="s">
         <v>77</v>
       </c>
-      <c r="F36" t="s">
-        <v>76</v>
-      </c>
       <c r="G36" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H36"/>
       <c r="I36"/>
       <c r="J36" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K36">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L36">
         <v>1</v>
       </c>
       <c r="M36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N36" t="s">
         <v>80</v>
@@ -2871,30 +2938,30 @@
         <v>64</v>
       </c>
       <c r="D37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E37" t="s">
+        <v>76</v>
+      </c>
+      <c r="F37" t="s">
         <v>77</v>
       </c>
-      <c r="F37" t="s">
-        <v>76</v>
-      </c>
       <c r="G37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H37"/>
       <c r="I37"/>
       <c r="J37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K37">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L37">
         <v>1</v>
       </c>
       <c r="M37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N37" t="s">
         <v>80</v>
@@ -2911,33 +2978,97 @@
         <v>66</v>
       </c>
       <c r="D38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E38" t="s">
+        <v>76</v>
+      </c>
+      <c r="F38" t="s">
         <v>77</v>
       </c>
-      <c r="F38" t="s">
-        <v>76</v>
-      </c>
       <c r="G38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H38"/>
       <c r="I38"/>
       <c r="J38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K38">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L38">
         <v>1</v>
       </c>
       <c r="M38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N38" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39">
+        <v>123456789</v>
+      </c>
+      <c r="B39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39"/>
+      <c r="E39" t="s">
+        <v>76</v>
+      </c>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39">
+        <v>1</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40">
+        <v>123456789</v>
+      </c>
+      <c r="B40" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40"/>
+      <c r="E40" t="s">
+        <v>76</v>
+      </c>
+      <c r="F40"/>
+      <c r="G40"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40"/>
+      <c r="K40">
+        <v>1</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>